<commit_message>
added pages to IG
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-MyPatient.xlsx
+++ b/output/StructureDefinition-MyPatient.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="367">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-05T15:53:09+01:00</t>
+    <t>2025-02-05T16:34:42+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -270,7 +270,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Patient[classCode=PAT]</t>
@@ -320,17 +320,10 @@
     <t>Resource.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">ele-1
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Patient.implicitRules</t>
   </si>
   <si>
@@ -350,9 +343,6 @@
     <t>Resource.implicitRules</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Patient.language</t>
   </si>
   <si>
@@ -430,6 +420,9 @@
     <t>DomainResource.contained</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>Patient.extension</t>
   </si>
   <si>
@@ -448,16 +441,6 @@
   </si>
   <si>
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
   </si>
   <si>
     <t>DomainResource.extension</t>
@@ -539,6 +522,9 @@
     <t>statusCode</t>
   </si>
   <si>
+    <t>n/a</t>
+  </si>
+  <si>
     <t>FiveWs.status</t>
   </si>
   <si>
@@ -589,10 +575,6 @@
     <t>People have (primary) ways to contact them in some way such as phone, email.</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-cpt-2:A system is required if a value is provided. {value.empty() or system.exists()}</t>
-  </si>
-  <si>
     <t>telecom</t>
   </si>
   <si>
@@ -730,9 +712,6 @@
   </si>
   <si>
     <t>This field contains a patient's most recent marital (civil) status.</t>
-  </si>
-  <si>
-    <t>Not all terminology uses fit this general pattern. In some cases, models should not use CodeableConcept and use Coding directly and provide their own structure for managing text, codings, translations and the relationship between elements and pre- and post-coordination.</t>
   </si>
   <si>
     <t>Most, if not all systems capture it.</t>
@@ -803,10 +782,6 @@
     <t>Many EHR systems have the capability to capture an image of the patient. Fits with newer social media usage too.</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-att-1:If the Attachment has data, it SHALL have a contentType {data.empty() or contentType.exists()}</t>
-  </si>
-  <si>
     <t>player[classCode=PSN|ANM and determinerCode=INSTANCE]/desc</t>
   </si>
   <si>
@@ -914,9 +889,6 @@
     <t>A name associated with the contact person.</t>
   </si>
   <si>
-    <t>Names may be changed, or repudiated, or people may have different names in different contexts. Names may be divided into parts of different type that have variable significance depending on context, though the division into parts does not always matter. With personal names, the different parts might or might not be imbued with some implicit meaning; various cultures associate different importance with the name parts and the degree to which systems must care about name parts around the world varies widely.</t>
-  </si>
-  <si>
     <t>Contact persons need to be identified by name, but it is uncommon to need details about multiple other names for that contact person.</t>
   </si>
   <si>
@@ -947,9 +919,6 @@
     <t>Address for the contact person.</t>
   </si>
   <si>
-    <t>Note: address is intended to describe postal addresses for administrative purposes, not to describe absolute geographical coordinates.  Postal addresses are often used as proxies for physical locations (also see the [Location](http://hl7.org/fhir/R4/location.html#) resource).</t>
-  </si>
-  <si>
     <t>Need to keep track where the contact person can be contacted per postal mail or visited.</t>
   </si>
   <si>
@@ -960,9 +929,6 @@
   </si>
   <si>
     <t>Administrative Gender - the gender that the contact person is considered to have for administration and record keeping purposes.</t>
-  </si>
-  <si>
-    <t>Note that FHIR strings SHALL NOT exceed 1MB in size</t>
   </si>
   <si>
     <t>Needed to address the person correctly.</t>
@@ -984,18 +950,11 @@
     <t>Organization on behalf of which the contact is acting or for which the contact is working.</t>
   </si>
   <si>
-    <t>References SHALL be a reference to an actual FHIR resource, and SHALL be resolveable (allowing for access control, temporary unavailability, etc.). Resolution can be either by retrieval from the URL, or, where applicable by resource type, by treating an absolute reference as a canonical URL and looking it up in a local registry/repository.</t>
-  </si>
-  <si>
     <t>For guardians or business related contacts, the organization is relevant.</t>
   </si>
   <si>
-    <t>ele-1
-pat-1</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ref-1:SHALL have a contained resource if a local reference is provided {reference.startsWith('#').not() or (reference.substring(1).trace('url') in %rootResource.contained.id.trace('ids'))}</t>
+    <t xml:space="preserve">pat-1
+</t>
   </si>
   <si>
     <t>scoper</t>
@@ -1017,18 +976,7 @@
     <t>The period during which this contact person or organization is valid to be contacted relating to this patient.</t>
   </si>
   <si>
-    <t>A Period specifies a range of time; the context of use will specify whether the entire range applies (e.g. "the patient was an inpatient of the hospital for this time range") or one value from the range applies (e.g. "give to the patient between these two times").
-Period is not used for a duration (a measure of elapsed time). See [Duration](http://hl7.org/fhir/R4/datatypes.html#Duration).</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-per-1:If present, start SHALL have a lower value than end {start.hasValue().not() or end.hasValue().not() or (start &lt;= end)}</t>
-  </si>
-  <si>
     <t>effectiveTime</t>
-  </si>
-  <si>
-    <t>DR</t>
   </si>
   <si>
     <t>Patient.communication</t>
@@ -1542,17 +1490,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="38.84375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="38.84375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.203125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="38.203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="50.0" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="48.09375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1561,27 +1509,27 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="78.75390625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="52.28125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="9.04296875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="77.9609375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="52.46484375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="153.5546875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="39.8515625" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="38.1328125" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="35.6015625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="151.51171875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="39.390625" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="33.05078125" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="41.1328125" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="36.4375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2035,13 +1983,13 @@
         <v>87</v>
       </c>
       <c r="AI4" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ4" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ4" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK4" t="s" s="2">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="AL4" t="s" s="2">
         <v>19</v>
@@ -2058,10 +2006,10 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -2084,16 +2032,16 @@
         <v>88</v>
       </c>
       <c r="K5" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="L5" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="M5" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="L5" t="s" s="2">
+      <c r="N5" t="s" s="2">
         <v>104</v>
-      </c>
-      <c r="M5" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N5" t="s" s="2">
-        <v>106</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
@@ -2143,7 +2091,7 @@
         <v>19</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>78</v>
@@ -2152,13 +2100,13 @@
         <v>87</v>
       </c>
       <c r="AI5" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ5" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ5" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK5" t="s" s="2">
-        <v>108</v>
+        <v>19</v>
       </c>
       <c r="AL5" t="s" s="2">
         <v>19</v>
@@ -2175,10 +2123,10 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -2201,16 +2149,16 @@
         <v>19</v>
       </c>
       <c r="K6" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="L6" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="M6" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="N6" t="s" s="2">
         <v>110</v>
-      </c>
-      <c r="L6" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="N6" t="s" s="2">
-        <v>113</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
@@ -2236,31 +2184,31 @@
         <v>19</v>
       </c>
       <c r="X6" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="Y6" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="Z6" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="AA6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF6" t="s" s="2">
         <v>114</v>
-      </c>
-      <c r="Y6" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="Z6" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="AA6" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB6" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC6" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD6" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF6" t="s" s="2">
-        <v>117</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>78</v>
@@ -2269,13 +2217,13 @@
         <v>87</v>
       </c>
       <c r="AI6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ6" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ6" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK6" t="s" s="2">
-        <v>108</v>
+        <v>19</v>
       </c>
       <c r="AL6" t="s" s="2">
         <v>19</v>
@@ -2292,14 +2240,14 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
@@ -2318,16 +2266,16 @@
         <v>19</v>
       </c>
       <c r="K7" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="L7" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="M7" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="N7" t="s" s="2">
         <v>120</v>
-      </c>
-      <c r="L7" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="M7" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="N7" t="s" s="2">
-        <v>123</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
@@ -2377,7 +2325,7 @@
         <v>19</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>78</v>
@@ -2386,13 +2334,13 @@
         <v>87</v>
       </c>
       <c r="AI7" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ7" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ7" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK7" t="s" s="2">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AL7" t="s" s="2">
         <v>19</v>
@@ -2409,14 +2357,14 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
@@ -2435,16 +2383,16 @@
         <v>19</v>
       </c>
       <c r="K8" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="L8" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="M8" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="N8" t="s" s="2">
         <v>128</v>
-      </c>
-      <c r="L8" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>130</v>
-      </c>
-      <c r="N8" t="s" s="2">
-        <v>131</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -2494,7 +2442,7 @@
         <v>19</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>78</v>
@@ -2509,7 +2457,7 @@
         <v>19</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="AL8" t="s" s="2">
         <v>19</v>
@@ -2526,14 +2474,14 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
@@ -2552,16 +2500,16 @@
         <v>19</v>
       </c>
       <c r="K9" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="L9" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="M9" t="s" s="2">
         <v>135</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="N9" t="s" s="2">
         <v>136</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="N9" t="s" s="2">
-        <v>138</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
@@ -2599,19 +2547,19 @@
         <v>19</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="AD9" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>78</v>
@@ -2620,13 +2568,13 @@
         <v>79</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="AL9" t="s" s="2">
         <v>19</v>
@@ -2643,14 +2591,14 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
@@ -2669,19 +2617,19 @@
         <v>19</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="O10" t="s" s="2">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="P10" t="s" s="2">
         <v>19</v>
@@ -2718,19 +2666,19 @@
         <v>19</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="AC10" t="s" s="2">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="AD10" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>78</v>
@@ -2739,13 +2687,13 @@
         <v>79</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="AL10" t="s" s="2">
         <v>19</v>
@@ -2762,10 +2710,10 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2788,17 +2736,17 @@
         <v>88</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="P11" t="s" s="2">
         <v>19</v>
@@ -2847,7 +2795,7 @@
         <v>19</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>78</v>
@@ -2856,22 +2804,22 @@
         <v>79</v>
       </c>
       <c r="AI11" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ11" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ11" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK11" t="s" s="2">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="AO11" t="s" s="2">
         <v>19</v>
@@ -2879,10 +2827,10 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2905,26 +2853,26 @@
         <v>88</v>
       </c>
       <c r="K12" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L12" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="M12" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="N12" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="O12" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="P12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="Q12" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="L12" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="N12" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="O12" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="P12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q12" t="s" s="2">
-        <v>164</v>
-      </c>
       <c r="R12" t="s" s="2">
         <v>19</v>
       </c>
@@ -2968,7 +2916,7 @@
         <v>19</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>78</v>
@@ -2977,19 +2925,19 @@
         <v>87</v>
       </c>
       <c r="AI12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ12" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ12" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK12" t="s" s="2">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AN12" t="s" s="2">
         <v>19</v>
@@ -3000,10 +2948,10 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -3026,19 +2974,19 @@
         <v>88</v>
       </c>
       <c r="K13" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="L13" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="M13" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="N13" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="O13" t="s" s="2">
         <v>168</v>
-      </c>
-      <c r="L13" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="N13" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="O13" t="s" s="2">
-        <v>172</v>
       </c>
       <c r="P13" t="s" s="2">
         <v>19</v>
@@ -3087,7 +3035,7 @@
         <v>19</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>78</v>
@@ -3096,22 +3044,22 @@
         <v>79</v>
       </c>
       <c r="AI13" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ13" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ13" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK13" t="s" s="2">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="AM13" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AO13" t="s" s="2">
         <v>19</v>
@@ -3119,10 +3067,10 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3145,19 +3093,19 @@
         <v>88</v>
       </c>
       <c r="K14" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="L14" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="M14" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="N14" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="O14" t="s" s="2">
         <v>177</v>
-      </c>
-      <c r="L14" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="N14" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="O14" t="s" s="2">
-        <v>181</v>
       </c>
       <c r="P14" t="s" s="2">
         <v>19</v>
@@ -3206,7 +3154,7 @@
         <v>19</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>78</v>
@@ -3215,22 +3163,22 @@
         <v>79</v>
       </c>
       <c r="AI14" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ14" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ14" t="s" s="2">
-        <v>182</v>
-      </c>
       <c r="AK14" t="s" s="2">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="AM14" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="AO14" t="s" s="2">
         <v>19</v>
@@ -3238,10 +3186,10 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3264,19 +3212,19 @@
         <v>88</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="O15" t="s" s="2">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="P15" t="s" s="2">
         <v>19</v>
@@ -3301,13 +3249,13 @@
         <v>19</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>19</v>
@@ -3325,7 +3273,7 @@
         <v>19</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>78</v>
@@ -3334,22 +3282,22 @@
         <v>87</v>
       </c>
       <c r="AI15" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ15" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ15" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK15" t="s" s="2">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AM15" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>19</v>
@@ -3357,10 +3305,10 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3383,19 +3331,19 @@
         <v>88</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>19</v>
@@ -3444,7 +3392,7 @@
         <v>19</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>78</v>
@@ -3453,33 +3401,33 @@
         <v>87</v>
       </c>
       <c r="AI16" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ16" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK16" t="s" s="2">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="AM16" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3502,19 +3450,19 @@
         <v>88</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>19</v>
@@ -3563,7 +3511,7 @@
         <v>19</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>78</v>
@@ -3572,22 +3520,22 @@
         <v>87</v>
       </c>
       <c r="AI17" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ17" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK17" t="s" s="2">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM17" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>19</v>
@@ -3595,10 +3543,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3621,19 +3569,19 @@
         <v>88</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="O18" t="s" s="2">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="P18" t="s" s="2">
         <v>19</v>
@@ -3682,7 +3630,7 @@
         <v>19</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>78</v>
@@ -3691,22 +3639,22 @@
         <v>79</v>
       </c>
       <c r="AI18" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ18" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ18" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK18" t="s" s="2">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="AM18" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>19</v>
@@ -3714,10 +3662,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3740,19 +3688,17 @@
         <v>19</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>228</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>19</v>
@@ -3777,13 +3723,13 @@
         <v>19</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="Z19" t="s" s="2">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AA19" t="s" s="2">
         <v>19</v>
@@ -3801,7 +3747,7 @@
         <v>19</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>78</v>
@@ -3810,22 +3756,22 @@
         <v>87</v>
       </c>
       <c r="AI19" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ19" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ19" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK19" t="s" s="2">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AM19" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>19</v>
@@ -3833,10 +3779,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3859,19 +3805,19 @@
         <v>19</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>19</v>
@@ -3920,7 +3866,7 @@
         <v>19</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>78</v>
@@ -3929,22 +3875,22 @@
         <v>87</v>
       </c>
       <c r="AI20" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ20" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ20" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK20" t="s" s="2">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>19</v>
@@ -3952,10 +3898,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3978,19 +3924,19 @@
         <v>19</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="O21" t="s" s="2">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="P21" t="s" s="2">
         <v>19</v>
@@ -4039,7 +3985,7 @@
         <v>19</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>78</v>
@@ -4048,22 +3994,22 @@
         <v>79</v>
       </c>
       <c r="AI21" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ21" t="s" s="2">
-        <v>250</v>
-      </c>
       <c r="AK21" t="s" s="2">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM21" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>19</v>
@@ -4071,10 +4017,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4097,19 +4043,19 @@
         <v>19</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>19</v>
@@ -4158,7 +4104,7 @@
         <v>19</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>78</v>
@@ -4167,16 +4113,16 @@
         <v>79</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>19</v>
@@ -4190,10 +4136,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4216,13 +4162,13 @@
         <v>19</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -4273,7 +4219,7 @@
         <v>19</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>78</v>
@@ -4288,7 +4234,7 @@
         <v>19</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>19</v>
@@ -4305,14 +4251,14 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
@@ -4331,16 +4277,16 @@
         <v>19</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L24" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="M24" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="N24" t="s" s="2">
         <v>136</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>138</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
@@ -4378,19 +4324,19 @@
         <v>19</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="AC24" t="s" s="2">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="AD24" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>78</v>
@@ -4399,13 +4345,13 @@
         <v>79</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>19</v>
@@ -4422,14 +4368,14 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4448,19 +4394,19 @@
         <v>88</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>19</v>
@@ -4509,7 +4455,7 @@
         <v>19</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>78</v>
@@ -4518,13 +4464,13 @@
         <v>79</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>19</v>
@@ -4541,10 +4487,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4567,19 +4513,17 @@
         <v>19</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>228</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>19</v>
@@ -4604,13 +4548,13 @@
         <v>19</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="Z26" t="s" s="2">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>19</v>
@@ -4628,7 +4572,7 @@
         <v>19</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>78</v>
@@ -4637,22 +4581,22 @@
         <v>79</v>
       </c>
       <c r="AI26" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ26" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ26" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK26" t="s" s="2">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>19</v>
@@ -4660,10 +4604,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4686,19 +4630,17 @@
         <v>19</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>285</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>19</v>
@@ -4747,7 +4689,7 @@
         <v>19</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>78</v>
@@ -4756,22 +4698,22 @@
         <v>87</v>
       </c>
       <c r="AI27" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ27" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ27" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK27" t="s" s="2">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>19</v>
@@ -4779,10 +4721,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4805,19 +4747,19 @@
         <v>19</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="N28" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="O28" t="s" s="2">
         <v>177</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="O28" t="s" s="2">
-        <v>181</v>
       </c>
       <c r="P28" t="s" s="2">
         <v>19</v>
@@ -4866,7 +4808,7 @@
         <v>19</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>78</v>
@@ -4875,22 +4817,22 @@
         <v>79</v>
       </c>
       <c r="AI28" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ28" t="s" s="2">
-        <v>182</v>
-      </c>
       <c r="AK28" t="s" s="2">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="AO28" t="s" s="2">
         <v>19</v>
@@ -4898,10 +4840,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4924,19 +4866,17 @@
         <v>19</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>296</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>19</v>
@@ -4985,7 +4925,7 @@
         <v>19</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -4994,22 +4934,22 @@
         <v>87</v>
       </c>
       <c r="AI29" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ29" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK29" t="s" s="2">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM29" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>19</v>
@@ -5017,10 +4957,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5043,19 +4983,17 @@
         <v>19</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>301</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="P30" t="s" s="2">
         <v>19</v>
@@ -5080,13 +5018,13 @@
         <v>19</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="Z30" t="s" s="2">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>19</v>
@@ -5104,7 +5042,7 @@
         <v>19</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>78</v>
@@ -5113,22 +5051,22 @@
         <v>87</v>
       </c>
       <c r="AI30" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ30" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK30" t="s" s="2">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="AO30" t="s" s="2">
         <v>19</v>
@@ -5136,10 +5074,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5162,19 +5100,17 @@
         <v>19</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>308</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>19</v>
@@ -5223,7 +5159,7 @@
         <v>19</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>78</v>
@@ -5232,22 +5168,22 @@
         <v>87</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>311</v>
+        <v>99</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="AO31" t="s" s="2">
         <v>19</v>
@@ -5255,10 +5191,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5281,17 +5217,15 @@
         <v>19</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>318</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
         <v>19</v>
@@ -5340,7 +5274,7 @@
         <v>19</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5349,22 +5283,22 @@
         <v>87</v>
       </c>
       <c r="AI32" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ32" t="s" s="2">
-        <v>319</v>
-      </c>
       <c r="AK32" t="s" s="2">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>321</v>
+        <v>19</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>19</v>
@@ -5372,10 +5306,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5398,19 +5332,19 @@
         <v>19</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="O33" t="s" s="2">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>19</v>
@@ -5459,7 +5393,7 @@
         <v>19</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>78</v>
@@ -5468,16 +5402,16 @@
         <v>79</v>
       </c>
       <c r="AI33" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ33" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ33" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK33" t="s" s="2">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>19</v>
@@ -5491,10 +5425,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5517,13 +5451,13 @@
         <v>19</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5574,7 +5508,7 @@
         <v>19</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>78</v>
@@ -5589,7 +5523,7 @@
         <v>19</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>19</v>
@@ -5606,14 +5540,14 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5632,16 +5566,16 @@
         <v>19</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L35" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="N35" t="s" s="2">
         <v>136</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>138</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5679,19 +5613,19 @@
         <v>19</v>
       </c>
       <c r="AB35" t="s" s="2">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="AC35" t="s" s="2">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="AD35" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>78</v>
@@ -5700,13 +5634,13 @@
         <v>79</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>19</v>
@@ -5723,14 +5657,14 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
@@ -5749,19 +5683,19 @@
         <v>88</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>19</v>
@@ -5810,7 +5744,7 @@
         <v>19</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>78</v>
@@ -5819,13 +5753,13 @@
         <v>79</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>19</v>
@@ -5842,10 +5776,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5868,19 +5802,19 @@
         <v>19</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>19</v>
@@ -5905,13 +5839,13 @@
         <v>19</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>19</v>
@@ -5929,7 +5863,7 @@
         <v>19</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>87</v>
@@ -5938,22 +5872,22 @@
         <v>87</v>
       </c>
       <c r="AI37" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ37" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ37" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK37" t="s" s="2">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>19</v>
@@ -5961,10 +5895,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5987,19 +5921,19 @@
         <v>19</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>19</v>
@@ -6048,7 +5982,7 @@
         <v>19</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
@@ -6057,22 +5991,22 @@
         <v>87</v>
       </c>
       <c r="AI38" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ38" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ38" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK38" t="s" s="2">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>19</v>
@@ -6080,14 +6014,14 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -6106,16 +6040,16 @@
         <v>19</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
@@ -6165,7 +6099,7 @@
         <v>19</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>78</v>
@@ -6174,22 +6108,22 @@
         <v>79</v>
       </c>
       <c r="AI39" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ39" t="s" s="2">
-        <v>311</v>
-      </c>
       <c r="AK39" t="s" s="2">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>19</v>
@@ -6197,10 +6131,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6223,19 +6157,19 @@
         <v>88</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="O40" t="s" s="2">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="P40" t="s" s="2">
         <v>19</v>
@@ -6284,7 +6218,7 @@
         <v>19</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>78</v>
@@ -6293,16 +6227,16 @@
         <v>87</v>
       </c>
       <c r="AI40" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ40" t="s" s="2">
-        <v>311</v>
-      </c>
       <c r="AK40" t="s" s="2">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>19</v>
@@ -6316,10 +6250,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6342,19 +6276,19 @@
         <v>88</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="O41" t="s" s="2">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>19</v>
@@ -6403,7 +6337,7 @@
         <v>19</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>78</v>
@@ -6412,16 +6346,16 @@
         <v>79</v>
       </c>
       <c r="AI41" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ41" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK41" t="s" s="2">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>19</v>
@@ -6435,10 +6369,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6461,13 +6395,13 @@
         <v>19</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -6518,7 +6452,7 @@
         <v>19</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>78</v>
@@ -6533,7 +6467,7 @@
         <v>19</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>19</v>
@@ -6550,14 +6484,14 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
@@ -6576,16 +6510,16 @@
         <v>19</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L43" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="N43" t="s" s="2">
         <v>136</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>138</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -6623,19 +6557,19 @@
         <v>19</v>
       </c>
       <c r="AB43" t="s" s="2">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="AC43" t="s" s="2">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="AD43" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>78</v>
@@ -6644,13 +6578,13 @@
         <v>79</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>19</v>
@@ -6667,14 +6601,14 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
@@ -6693,19 +6627,19 @@
         <v>88</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="O44" t="s" s="2">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>19</v>
@@ -6754,7 +6688,7 @@
         <v>19</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>78</v>
@@ -6763,13 +6697,13 @@
         <v>79</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>19</v>
@@ -6786,10 +6720,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6812,16 +6746,16 @@
         <v>88</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -6871,7 +6805,7 @@
         <v>19</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>87</v>
@@ -6880,22 +6814,22 @@
         <v>87</v>
       </c>
       <c r="AI45" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ45" t="s" s="2">
-        <v>311</v>
-      </c>
       <c r="AK45" t="s" s="2">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>19</v>
@@ -6903,10 +6837,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6929,17 +6863,15 @@
         <v>88</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>301</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
         <v>19</v>
@@ -6964,13 +6896,13 @@
         <v>19</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="Z46" t="s" s="2">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="AA46" t="s" s="2">
         <v>19</v>
@@ -6988,7 +6920,7 @@
         <v>19</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>87</v>
@@ -6997,16 +6929,16 @@
         <v>87</v>
       </c>
       <c r="AI46" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AJ46" t="s" s="2">
-        <v>100</v>
-      </c>
       <c r="AK46" t="s" s="2">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>19</v>

</xml_diff>

<commit_message>
added corrections to IG
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-MyPatient.xlsx
+++ b/output/StructureDefinition-MyPatient.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="382">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-05T16:34:42+01:00</t>
+    <t>2025-02-05T17:06:32+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -69,7 +69,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Berlin Institute of Health (http://example.org/example-publisher)</t>
+    <t>Berlin Institute of Health (https://www.bihealth.org)</t>
   </si>
   <si>
     <t>Jurisdiction</t>
@@ -270,7 +270,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
+dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}</t>
   </si>
   <si>
     <t>Patient[classCode=PAT]</t>
@@ -320,10 +320,17 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>Patient.implicitRules</t>
   </si>
   <si>
@@ -343,6 +350,9 @@
     <t>Resource.implicitRules</t>
   </si>
   <si>
+    <t>n/a</t>
+  </si>
+  <si>
     <t>Patient.language</t>
   </si>
   <si>
@@ -420,9 +430,6 @@
     <t>DomainResource.contained</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Patient.extension</t>
   </si>
   <si>
@@ -441,6 +448,16 @@
   </si>
   <si>
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
   <si>
     <t>DomainResource.extension</t>
@@ -522,9 +539,6 @@
     <t>statusCode</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>FiveWs.status</t>
   </si>
   <si>
@@ -575,6 +589,10 @@
     <t>People have (primary) ways to contact them in some way such as phone, email.</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+cpt-2:A system is required if a value is provided. {value.empty() or system.exists()}</t>
+  </si>
+  <si>
     <t>telecom</t>
   </si>
   <si>
@@ -712,6 +730,9 @@
   </si>
   <si>
     <t>This field contains a patient's most recent marital (civil) status.</t>
+  </si>
+  <si>
+    <t>Not all terminology uses fit this general pattern. In some cases, models should not use CodeableConcept and use Coding directly and provide their own structure for managing text, codings, translations and the relationship between elements and pre- and post-coordination.</t>
   </si>
   <si>
     <t>Most, if not all systems capture it.</t>
@@ -782,6 +803,10 @@
     <t>Many EHR systems have the capability to capture an image of the patient. Fits with newer social media usage too.</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+att-1:If the Attachment has data, it SHALL have a contentType {data.empty() or contentType.exists()}</t>
+  </si>
+  <si>
     <t>player[classCode=PSN|ANM and determinerCode=INSTANCE]/desc</t>
   </si>
   <si>
@@ -889,6 +914,9 @@
     <t>A name associated with the contact person.</t>
   </si>
   <si>
+    <t>Names may be changed, or repudiated, or people may have different names in different contexts. Names may be divided into parts of different type that have variable significance depending on context, though the division into parts does not always matter. With personal names, the different parts might or might not be imbued with some implicit meaning; various cultures associate different importance with the name parts and the degree to which systems must care about name parts around the world varies widely.</t>
+  </si>
+  <si>
     <t>Contact persons need to be identified by name, but it is uncommon to need details about multiple other names for that contact person.</t>
   </si>
   <si>
@@ -919,6 +947,9 @@
     <t>Address for the contact person.</t>
   </si>
   <si>
+    <t>Note: address is intended to describe postal addresses for administrative purposes, not to describe absolute geographical coordinates.  Postal addresses are often used as proxies for physical locations (also see the [Location](http://hl7.org/fhir/R4/location.html#) resource).</t>
+  </si>
+  <si>
     <t>Need to keep track where the contact person can be contacted per postal mail or visited.</t>
   </si>
   <si>
@@ -929,6 +960,9 @@
   </si>
   <si>
     <t>Administrative Gender - the gender that the contact person is considered to have for administration and record keeping purposes.</t>
+  </si>
+  <si>
+    <t>Note that FHIR strings SHALL NOT exceed 1MB in size</t>
   </si>
   <si>
     <t>Needed to address the person correctly.</t>
@@ -950,11 +984,18 @@
     <t>Organization on behalf of which the contact is acting or for which the contact is working.</t>
   </si>
   <si>
+    <t>References SHALL be a reference to an actual FHIR resource, and SHALL be resolveable (allowing for access control, temporary unavailability, etc.). Resolution can be either by retrieval from the URL, or, where applicable by resource type, by treating an absolute reference as a canonical URL and looking it up in a local registry/repository.</t>
+  </si>
+  <si>
     <t>For guardians or business related contacts, the organization is relevant.</t>
   </si>
   <si>
-    <t xml:space="preserve">pat-1
-</t>
+    <t>ele-1
+pat-1</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ref-1:SHALL have a contained resource if a local reference is provided {reference.startsWith('#').not() or (reference.substring(1).trace('url') in %rootResource.contained.id.trace('ids'))}</t>
   </si>
   <si>
     <t>scoper</t>
@@ -976,7 +1017,18 @@
     <t>The period during which this contact person or organization is valid to be contacted relating to this patient.</t>
   </si>
   <si>
+    <t>A Period specifies a range of time; the context of use will specify whether the entire range applies (e.g. "the patient was an inpatient of the hospital for this time range") or one value from the range applies (e.g. "give to the patient between these two times").
+Period is not used for a duration (a measure of elapsed time). See [Duration](http://hl7.org/fhir/R4/datatypes.html#Duration).</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+per-1:If present, start SHALL have a lower value than end {start.hasValue().not() or end.hasValue().not() or (start &lt;= end)}</t>
+  </si>
+  <si>
     <t>effectiveTime</t>
+  </si>
+  <si>
+    <t>DR</t>
   </si>
   <si>
     <t>Patient.communication</t>
@@ -1490,17 +1542,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="38.203125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="38.203125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.84375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="38.84375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="48.09375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="50.0" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1509,27 +1561,27 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.04296875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="77.9609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="52.46484375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="78.75390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="52.28125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="151.51171875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="39.390625" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="33.05078125" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="41.1328125" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="36.4375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="153.5546875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="39.8515625" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="32.84375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="38.1328125" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="35.6015625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1983,13 +2035,13 @@
         <v>87</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK4" t="s" s="2">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="AL4" t="s" s="2">
         <v>19</v>
@@ -2006,10 +2058,10 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -2032,16 +2084,16 @@
         <v>88</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N5" t="s" s="2">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
@@ -2091,7 +2143,7 @@
         <v>19</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>78</v>
@@ -2100,13 +2152,13 @@
         <v>87</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="AL5" t="s" s="2">
         <v>19</v>
@@ -2123,10 +2175,10 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -2149,16 +2201,16 @@
         <v>19</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="N6" t="s" s="2">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
@@ -2184,13 +2236,13 @@
         <v>19</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AA6" t="s" s="2">
         <v>19</v>
@@ -2208,7 +2260,7 @@
         <v>19</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>78</v>
@@ -2217,13 +2269,13 @@
         <v>87</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="AL6" t="s" s="2">
         <v>19</v>
@@ -2240,14 +2292,14 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
@@ -2266,16 +2318,16 @@
         <v>19</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="N7" t="s" s="2">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
@@ -2325,7 +2377,7 @@
         <v>19</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>78</v>
@@ -2334,13 +2386,13 @@
         <v>87</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AL7" t="s" s="2">
         <v>19</v>
@@ -2357,14 +2409,14 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
@@ -2383,16 +2435,16 @@
         <v>19</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="N8" t="s" s="2">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -2442,7 +2494,7 @@
         <v>19</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>78</v>
@@ -2457,7 +2509,7 @@
         <v>19</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="AL8" t="s" s="2">
         <v>19</v>
@@ -2474,14 +2526,14 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
@@ -2500,16 +2552,16 @@
         <v>19</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="N9" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
@@ -2547,19 +2599,19 @@
         <v>19</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="AD9" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>78</v>
@@ -2568,13 +2620,13 @@
         <v>79</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="AL9" t="s" s="2">
         <v>19</v>
@@ -2591,14 +2643,14 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
@@ -2617,19 +2669,19 @@
         <v>19</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O10" t="s" s="2">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="P10" t="s" s="2">
         <v>19</v>
@@ -2666,19 +2718,19 @@
         <v>19</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="AC10" t="s" s="2">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="AD10" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>78</v>
@@ -2687,13 +2739,13 @@
         <v>79</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="AL10" t="s" s="2">
         <v>19</v>
@@ -2710,10 +2762,10 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2736,17 +2788,17 @@
         <v>88</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="P11" t="s" s="2">
         <v>19</v>
@@ -2795,7 +2847,7 @@
         <v>19</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>78</v>
@@ -2804,22 +2856,22 @@
         <v>79</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="AO11" t="s" s="2">
         <v>19</v>
@@ -2827,10 +2879,10 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2853,70 +2905,70 @@
         <v>88</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="O12" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="P12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="Q12" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="R12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="S12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="T12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="U12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="V12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="W12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="X12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="Y12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="Z12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AA12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF12" t="s" s="2">
         <v>158</v>
-      </c>
-      <c r="P12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q12" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="R12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE12" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF12" t="s" s="2">
-        <v>153</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>78</v>
@@ -2925,19 +2977,19 @@
         <v>87</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="AN12" t="s" s="2">
         <v>19</v>
@@ -2948,10 +3000,10 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -2974,19 +3026,19 @@
         <v>88</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="O13" t="s" s="2">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="P13" t="s" s="2">
         <v>19</v>
@@ -3035,7 +3087,7 @@
         <v>19</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>78</v>
@@ -3044,22 +3096,22 @@
         <v>79</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="AM13" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="AO13" t="s" s="2">
         <v>19</v>
@@ -3067,10 +3119,10 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3093,19 +3145,19 @@
         <v>88</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="O14" t="s" s="2">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="P14" t="s" s="2">
         <v>19</v>
@@ -3154,7 +3206,7 @@
         <v>19</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>78</v>
@@ -3163,22 +3215,22 @@
         <v>79</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>99</v>
+        <v>182</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="AM14" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AO14" t="s" s="2">
         <v>19</v>
@@ -3186,10 +3238,10 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3212,19 +3264,19 @@
         <v>88</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="O15" t="s" s="2">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="P15" t="s" s="2">
         <v>19</v>
@@ -3249,31 +3301,31 @@
         <v>19</v>
       </c>
       <c r="X15" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="Y15" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="Z15" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="AA15" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB15" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC15" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD15" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE15" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF15" t="s" s="2">
         <v>186</v>
-      </c>
-      <c r="Y15" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="Z15" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="AA15" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB15" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC15" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD15" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE15" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF15" t="s" s="2">
-        <v>181</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>78</v>
@@ -3282,22 +3334,22 @@
         <v>87</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="AM15" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>19</v>
@@ -3305,10 +3357,10 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3331,19 +3383,19 @@
         <v>88</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>19</v>
@@ -3392,7 +3444,7 @@
         <v>19</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>78</v>
@@ -3401,33 +3453,33 @@
         <v>87</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="AM16" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3450,19 +3502,19 @@
         <v>88</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>19</v>
@@ -3511,7 +3563,7 @@
         <v>19</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>78</v>
@@ -3520,22 +3572,22 @@
         <v>87</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM17" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>19</v>
@@ -3543,10 +3595,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3569,19 +3621,19 @@
         <v>88</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="O18" t="s" s="2">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="P18" t="s" s="2">
         <v>19</v>
@@ -3630,7 +3682,7 @@
         <v>19</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>78</v>
@@ -3639,22 +3691,22 @@
         <v>79</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="AM18" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>19</v>
@@ -3662,10 +3714,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3688,17 +3740,19 @@
         <v>19</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="N19" s="2"/>
+        <v>227</v>
+      </c>
+      <c r="N19" t="s" s="2">
+        <v>228</v>
+      </c>
       <c r="O19" t="s" s="2">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>19</v>
@@ -3723,31 +3777,31 @@
         <v>19</v>
       </c>
       <c r="X19" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="Y19" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="Z19" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AA19" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AB19" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AC19" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AD19" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AE19" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="AF19" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="Y19" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="Z19" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="AA19" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB19" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC19" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD19" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE19" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF19" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>78</v>
@@ -3756,22 +3810,22 @@
         <v>87</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="AM19" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>19</v>
@@ -3779,10 +3833,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3805,19 +3859,19 @@
         <v>19</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>19</v>
@@ -3866,7 +3920,7 @@
         <v>19</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>78</v>
@@ -3875,22 +3929,22 @@
         <v>87</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>19</v>
@@ -3898,10 +3952,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3924,19 +3978,19 @@
         <v>19</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="O21" t="s" s="2">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="P21" t="s" s="2">
         <v>19</v>
@@ -3985,7 +4039,7 @@
         <v>19</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>78</v>
@@ -3994,22 +4048,22 @@
         <v>79</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>99</v>
+        <v>250</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM21" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>19</v>
@@ -4017,10 +4071,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4043,19 +4097,19 @@
         <v>19</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>19</v>
@@ -4104,7 +4158,7 @@
         <v>19</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>78</v>
@@ -4113,16 +4167,16 @@
         <v>79</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>19</v>
@@ -4136,10 +4190,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4162,13 +4216,13 @@
         <v>19</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -4219,7 +4273,7 @@
         <v>19</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>78</v>
@@ -4234,7 +4288,7 @@
         <v>19</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>19</v>
@@ -4251,14 +4305,14 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
@@ -4277,16 +4331,16 @@
         <v>19</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
@@ -4324,19 +4378,19 @@
         <v>19</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="AC24" t="s" s="2">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="AD24" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>78</v>
@@ -4345,13 +4399,13 @@
         <v>79</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>161</v>
+        <v>101</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>19</v>
@@ -4368,14 +4422,14 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4394,19 +4448,19 @@
         <v>88</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>19</v>
@@ -4455,7 +4509,7 @@
         <v>19</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>78</v>
@@ -4464,13 +4518,13 @@
         <v>79</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>19</v>
@@ -4487,10 +4541,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4513,17 +4567,19 @@
         <v>19</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="N26" s="2"/>
+        <v>276</v>
+      </c>
+      <c r="N26" t="s" s="2">
+        <v>228</v>
+      </c>
       <c r="O26" t="s" s="2">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>19</v>
@@ -4548,13 +4604,13 @@
         <v>19</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="Z26" t="s" s="2">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>19</v>
@@ -4572,7 +4628,7 @@
         <v>19</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>78</v>
@@ -4581,22 +4637,22 @@
         <v>79</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>19</v>
@@ -4604,10 +4660,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4630,17 +4686,19 @@
         <v>19</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="N27" s="2"/>
+        <v>284</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>285</v>
+      </c>
       <c r="O27" t="s" s="2">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>19</v>
@@ -4689,7 +4747,7 @@
         <v>19</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>78</v>
@@ -4698,22 +4756,22 @@
         <v>87</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>19</v>
@@ -4721,10 +4779,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4747,19 +4805,19 @@
         <v>19</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="P28" t="s" s="2">
         <v>19</v>
@@ -4808,7 +4866,7 @@
         <v>19</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>78</v>
@@ -4817,22 +4875,22 @@
         <v>79</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>99</v>
+        <v>182</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="AO28" t="s" s="2">
         <v>19</v>
@@ -4840,10 +4898,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4866,17 +4924,19 @@
         <v>19</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="N29" s="2"/>
+        <v>295</v>
+      </c>
+      <c r="N29" t="s" s="2">
+        <v>296</v>
+      </c>
       <c r="O29" t="s" s="2">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>19</v>
@@ -4925,7 +4985,7 @@
         <v>19</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -4934,22 +4994,22 @@
         <v>87</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM29" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>19</v>
@@ -4957,10 +5017,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4983,17 +5043,19 @@
         <v>19</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="N30" s="2"/>
+        <v>300</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>301</v>
+      </c>
       <c r="O30" t="s" s="2">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="P30" t="s" s="2">
         <v>19</v>
@@ -5018,13 +5080,13 @@
         <v>19</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="Z30" t="s" s="2">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>19</v>
@@ -5042,7 +5104,7 @@
         <v>19</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>78</v>
@@ -5051,22 +5113,22 @@
         <v>87</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="AO30" t="s" s="2">
         <v>19</v>
@@ -5074,10 +5136,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5100,17 +5162,19 @@
         <v>19</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="N31" s="2"/>
+        <v>307</v>
+      </c>
+      <c r="N31" t="s" s="2">
+        <v>308</v>
+      </c>
       <c r="O31" t="s" s="2">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>19</v>
@@ -5159,7 +5223,7 @@
         <v>19</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>78</v>
@@ -5168,22 +5232,22 @@
         <v>87</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>99</v>
+        <v>311</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="AO31" t="s" s="2">
         <v>19</v>
@@ -5191,10 +5255,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5217,15 +5281,17 @@
         <v>19</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="N32" s="2"/>
+        <v>317</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>318</v>
+      </c>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
         <v>19</v>
@@ -5274,7 +5340,7 @@
         <v>19</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5283,22 +5349,22 @@
         <v>87</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>99</v>
+        <v>319</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>306</v>
+        <v>320</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>19</v>
+        <v>321</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>19</v>
@@ -5306,10 +5372,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5332,19 +5398,19 @@
         <v>19</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>309</v>
+        <v>324</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="O33" t="s" s="2">
-        <v>311</v>
+        <v>326</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>19</v>
@@ -5393,7 +5459,7 @@
         <v>19</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>78</v>
@@ -5402,16 +5468,16 @@
         <v>79</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>312</v>
+        <v>327</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>313</v>
+        <v>328</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>19</v>
@@ -5425,10 +5491,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5451,13 +5517,13 @@
         <v>19</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5508,7 +5574,7 @@
         <v>19</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>78</v>
@@ -5523,7 +5589,7 @@
         <v>19</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>19</v>
@@ -5540,14 +5606,14 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>315</v>
+        <v>330</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>315</v>
+        <v>330</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5566,16 +5632,16 @@
         <v>19</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5613,19 +5679,19 @@
         <v>19</v>
       </c>
       <c r="AB35" t="s" s="2">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="AC35" t="s" s="2">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="AD35" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>78</v>
@@ -5634,13 +5700,13 @@
         <v>79</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>161</v>
+        <v>101</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>19</v>
@@ -5657,14 +5723,14 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
@@ -5683,19 +5749,19 @@
         <v>88</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>19</v>
@@ -5744,7 +5810,7 @@
         <v>19</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>78</v>
@@ -5753,13 +5819,13 @@
         <v>79</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>19</v>
@@ -5776,10 +5842,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5802,19 +5868,19 @@
         <v>19</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>321</v>
+        <v>336</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>19</v>
@@ -5839,13 +5905,13 @@
         <v>19</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>19</v>
@@ -5863,7 +5929,7 @@
         <v>19</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>87</v>
@@ -5872,22 +5938,22 @@
         <v>87</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>323</v>
+        <v>338</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>19</v>
@@ -5895,10 +5961,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5921,19 +5987,19 @@
         <v>19</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>329</v>
+        <v>344</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>19</v>
@@ -5982,7 +6048,7 @@
         <v>19</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
@@ -5991,22 +6057,22 @@
         <v>87</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>332</v>
+        <v>347</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>19</v>
@@ -6014,14 +6080,14 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>334</v>
+        <v>349</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -6040,16 +6106,16 @@
         <v>19</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>336</v>
+        <v>351</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>338</v>
+        <v>353</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
@@ -6099,7 +6165,7 @@
         <v>19</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>78</v>
@@ -6108,22 +6174,22 @@
         <v>79</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>99</v>
+        <v>311</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>339</v>
+        <v>354</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>19</v>
@@ -6131,10 +6197,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>341</v>
+        <v>356</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>341</v>
+        <v>356</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6157,19 +6223,19 @@
         <v>88</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>342</v>
+        <v>357</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>343</v>
+        <v>358</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="O40" t="s" s="2">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="P40" t="s" s="2">
         <v>19</v>
@@ -6218,7 +6284,7 @@
         <v>19</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>341</v>
+        <v>356</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>78</v>
@@ -6227,16 +6293,16 @@
         <v>87</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>99</v>
+        <v>311</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>346</v>
+        <v>361</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>19</v>
@@ -6250,10 +6316,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6276,19 +6342,19 @@
         <v>88</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>348</v>
+        <v>363</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>349</v>
+        <v>364</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="O41" t="s" s="2">
-        <v>351</v>
+        <v>366</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>19</v>
@@ -6337,7 +6403,7 @@
         <v>19</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>78</v>
@@ -6346,16 +6412,16 @@
         <v>79</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>352</v>
+        <v>367</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>19</v>
@@ -6369,10 +6435,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>353</v>
+        <v>368</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>353</v>
+        <v>368</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6395,13 +6461,13 @@
         <v>19</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -6452,7 +6518,7 @@
         <v>19</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>78</v>
@@ -6467,7 +6533,7 @@
         <v>19</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>19</v>
@@ -6484,14 +6550,14 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>354</v>
+        <v>369</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>354</v>
+        <v>369</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
@@ -6510,16 +6576,16 @@
         <v>19</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -6557,19 +6623,19 @@
         <v>19</v>
       </c>
       <c r="AB43" t="s" s="2">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="AC43" t="s" s="2">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="AD43" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>78</v>
@@ -6578,13 +6644,13 @@
         <v>79</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>161</v>
+        <v>101</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>19</v>
@@ -6601,14 +6667,14 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
@@ -6627,19 +6693,19 @@
         <v>88</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O44" t="s" s="2">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>19</v>
@@ -6688,7 +6754,7 @@
         <v>19</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>78</v>
@@ -6697,13 +6763,13 @@
         <v>79</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>19</v>
@@ -6720,10 +6786,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>356</v>
+        <v>371</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>356</v>
+        <v>371</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6746,16 +6812,16 @@
         <v>88</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>357</v>
+        <v>372</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>358</v>
+        <v>373</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>359</v>
+        <v>374</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>360</v>
+        <v>375</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -6805,7 +6871,7 @@
         <v>19</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>356</v>
+        <v>371</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>87</v>
@@ -6814,22 +6880,22 @@
         <v>87</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>99</v>
+        <v>311</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>361</v>
+        <v>376</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>19</v>
@@ -6837,10 +6903,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>362</v>
+        <v>377</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>362</v>
+        <v>377</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6863,15 +6929,17 @@
         <v>88</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>363</v>
+        <v>378</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="N46" s="2"/>
+        <v>379</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>301</v>
+      </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
         <v>19</v>
@@ -6896,13 +6964,13 @@
         <v>19</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>364</v>
+        <v>379</v>
       </c>
       <c r="Z46" t="s" s="2">
-        <v>365</v>
+        <v>380</v>
       </c>
       <c r="AA46" t="s" s="2">
         <v>19</v>
@@ -6920,7 +6988,7 @@
         <v>19</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>362</v>
+        <v>377</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>87</v>
@@ -6929,16 +6997,16 @@
         <v>87</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>366</v>
+        <v>381</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>19</v>

</xml_diff>